<commit_message>
expanding manual testing spreadsheet
</commit_message>
<xml_diff>
--- a/BoardgameNerd/test/manualTests.xlsx
+++ b/BoardgameNerd/test/manualTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierluca/personal local/Work/Learn/CodeInstitute/workspace/BoardgameNerd/BoardgameNerd/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665D016F-7523-8046-81C1-CE72A87DA079}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF25EB4-0F32-CE45-ACD4-070D9210FAF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="17540" xr2:uid="{3B2D3A10-B4C2-C143-A6C2-842FD9F46DA7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="51">
   <si>
     <t>Validations</t>
   </si>
@@ -251,9 +251,6 @@
     </r>
   </si>
   <si>
-    <t>Collections.html</t>
-  </si>
-  <si>
     <t>Carousels slide correctly</t>
   </si>
   <si>
@@ -279,6 +276,15 @@
   </si>
   <si>
     <t>Empty Search are showing message</t>
+  </si>
+  <si>
+    <t>Collection.html</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>all .py Files are PEP8 compliant</t>
   </si>
 </sst>
 </file>
@@ -1002,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A56C59-A709-824B-A8C0-8BBDF3C895BA}">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:M18"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1119,7 +1125,7 @@
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
@@ -1140,231 +1146,197 @@
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13" ht="20" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="1:13" ht="20" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10" t="s">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-    </row>
-    <row r="9" spans="1:13" ht="28" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2" t="s">
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="1:13" ht="28" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-    </row>
-    <row r="10" spans="1:13" ht="48" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+    </row>
+    <row r="12" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="36" t="s">
+      <c r="F12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="38"/>
-    </row>
-    <row r="11" spans="1:13" ht="48" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="38"/>
+    </row>
+    <row r="13" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="B13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="39" t="s">
+      <c r="J13" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="41"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="41"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-    </row>
-    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+    </row>
+    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="14"/>
-    </row>
-    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>19</v>
@@ -1397,9 +1369,9 @@
       <c r="L16" s="13"/>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>19</v>
@@ -1426,15 +1398,15 @@
         <v>19</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="14"/>
     </row>
-    <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>19</v>
@@ -1467,9 +1439,9 @@
       <c r="L18" s="13"/>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>19</v>
@@ -1502,178 +1474,178 @@
       <c r="L19" s="13"/>
       <c r="M19" s="14"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
+    <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="14"/>
+    </row>
+    <row r="21" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="14"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J22" s="12" t="s">
+      <c r="B24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="14"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="14"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-    </row>
-    <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+    </row>
+    <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="14"/>
-    </row>
-    <row r="26" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J26" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="14"/>
-    </row>
-    <row r="27" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>19</v>
@@ -1708,7 +1680,7 @@
     </row>
     <row r="28" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>19</v>
@@ -1741,111 +1713,111 @@
       <c r="L28" s="13"/>
       <c r="M28" s="14"/>
     </row>
-    <row r="29" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-    </row>
-    <row r="31" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+    <row r="29" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="14"/>
+    </row>
+    <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="14"/>
+    </row>
+    <row r="31" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+    </row>
+    <row r="33" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="14"/>
-    </row>
-    <row r="32" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="14"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>19</v>
@@ -1878,154 +1850,227 @@
       <c r="L33" s="13"/>
       <c r="M33" s="14"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="16"/>
-    </row>
-    <row r="35" spans="1:13" ht="20" x14ac:dyDescent="0.2">
-      <c r="A35" s="24" t="s">
+    <row r="34" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="14"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="14"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+    </row>
+    <row r="37" spans="1:13" ht="20" x14ac:dyDescent="0.2">
+      <c r="A37" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="27" t="s">
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="K35" s="28"/>
-      <c r="L35" s="28"/>
-      <c r="M35" s="29"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1" t="s">
+      <c r="K37" s="28"/>
+      <c r="L37" s="28"/>
+      <c r="M37" s="29"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F36" s="30"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="32"/>
-    </row>
-    <row r="37" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+      <c r="F38" s="30"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="32"/>
+    </row>
+    <row r="39" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E37" s="4" t="s">
+      <c r="B39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F37" s="18"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="33" t="s">
+      <c r="F39" s="18"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="K37" s="34"/>
-      <c r="L37" s="34"/>
-      <c r="M37" s="35"/>
-    </row>
-    <row r="38" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+      <c r="K39" s="34"/>
+      <c r="L39" s="34"/>
+      <c r="M39" s="35"/>
+    </row>
+    <row r="40" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E38" s="4" t="s">
+      <c r="B40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="21"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="33" t="s">
+      <c r="F40" s="21"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="K38" s="34"/>
-      <c r="L38" s="34"/>
-      <c r="M38" s="35"/>
+      <c r="K40" s="34"/>
+      <c r="L40" s="34"/>
+      <c r="M40" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="F37:I38"/>
-    <mergeCell ref="A30:M30"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="J33:M33"/>
-    <mergeCell ref="A34:M34"/>
-    <mergeCell ref="A35:I35"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="F36:K36"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="A29:M29"/>
+  <mergeCells count="48">
     <mergeCell ref="J19:M19"/>
-    <mergeCell ref="A23:M23"/>
-    <mergeCell ref="A24:M24"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="A20:M20"/>
-    <mergeCell ref="A21:M21"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="J20:M20"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:I7"/>
     <mergeCell ref="J6:M7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="F39:I40"/>
+    <mergeCell ref="A32:M32"/>
+    <mergeCell ref="J33:M33"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="A36:M36"/>
+    <mergeCell ref="A37:I37"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="F38:K38"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="A31:M31"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="A25:M25"/>
+    <mergeCell ref="A26:M26"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="A22:M22"/>
+    <mergeCell ref="A23:M23"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:I9"/>
+    <mergeCell ref="J8:M9"/>
+    <mergeCell ref="A10:I10"/>
     <mergeCell ref="J10:M10"/>
     <mergeCell ref="J11:M11"/>
-    <mergeCell ref="A12:M12"/>
-    <mergeCell ref="A13:M13"/>
-    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="A14:M14"/>
+    <mergeCell ref="A15:M15"/>
+    <mergeCell ref="J16:M16"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:I5"/>
     <mergeCell ref="J4:M5"/>
@@ -2035,7 +2080,7 @@
     <mergeCell ref="B2:I3"/>
     <mergeCell ref="J2:M3"/>
   </mergeCells>
-  <conditionalFormatting sqref="B10:I11 B37:E38 B14:I19">
+  <conditionalFormatting sqref="B12:I13 B39:E40 B16:I21">
     <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"Poor"</formula>
     </cfRule>
@@ -2046,7 +2091,7 @@
       <formula>"Good"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25:I28">
+  <conditionalFormatting sqref="B27:I30">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"Poor"</formula>
     </cfRule>
@@ -2057,7 +2102,7 @@
       <formula>"Good"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31:I33">
+  <conditionalFormatting sqref="B33:I35">
     <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"Poor"</formula>
     </cfRule>
@@ -2068,7 +2113,7 @@
       <formula>"Good"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B22:I22">
+  <conditionalFormatting sqref="B24:I24">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Poor"</formula>
     </cfRule>

</xml_diff>

<commit_message>
adding images for 404 and 500
</commit_message>
<xml_diff>
--- a/BoardgameNerd/test/manualTests.xlsx
+++ b/BoardgameNerd/test/manualTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierluca/personal local/Work/Learn/CodeInstitute/workspace/BoardgameNerd/BoardgameNerd/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF25EB4-0F32-CE45-ACD4-070D9210FAF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3474DB-D9A0-7949-8D6D-DB2196DEC24D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="17540" xr2:uid="{3B2D3A10-B4C2-C143-A6C2-842FD9F46DA7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="63">
   <si>
     <t>Validations</t>
   </si>
@@ -165,13 +165,7 @@
     </r>
   </si>
   <si>
-    <t>INDEX.html</t>
-  </si>
-  <si>
     <t>Links / URLs work</t>
-  </si>
-  <si>
-    <t>Images work</t>
   </si>
   <si>
     <t>Renders as expected</t>
@@ -225,9 +219,6 @@
 responsiveness?</t>
   </si>
   <si>
-    <t>SEARCH.html</t>
-  </si>
-  <si>
     <t>warning related to extension not validable</t>
   </si>
   <si>
@@ -266,9 +257,6 @@
     <t>Features Section Renders correctly</t>
   </si>
   <si>
-    <t>NAV BAR</t>
-  </si>
-  <si>
     <t>Redirect Correctly</t>
   </si>
   <si>
@@ -285,6 +273,54 @@
   </si>
   <si>
     <t>all .py Files are PEP8 compliant</t>
+  </si>
+  <si>
+    <t>Navigation Bar</t>
+  </si>
+  <si>
+    <t>Search.html</t>
+  </si>
+  <si>
+    <t>Index.html</t>
+  </si>
+  <si>
+    <t>Detail.html</t>
+  </si>
+  <si>
+    <t>Add to Collection Work</t>
+  </si>
+  <si>
+    <t>Spinner</t>
+  </si>
+  <si>
+    <t>shows when supposed</t>
+  </si>
+  <si>
+    <t>Toast</t>
+  </si>
+  <si>
+    <t>edit/remove Games</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Wrong Password or User are detected</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>User Can Register</t>
+  </si>
+  <si>
+    <t>Esisting Users or Password are detected</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>empty collections are showing messages</t>
   </si>
 </sst>
 </file>
@@ -613,7 +649,196 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="39">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1008,10 +1233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A56C59-A709-824B-A8C0-8BBDF3C895BA}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:I7"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1053,7 +1278,7 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
@@ -1089,7 +1314,7 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
@@ -1125,7 +1350,7 @@
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
@@ -1148,7 +1373,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>7</v>
@@ -1161,7 +1386,7 @@
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
@@ -1261,7 +1486,7 @@
         <v>19</v>
       </c>
       <c r="J12" s="36" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K12" s="37"/>
       <c r="L12" s="37"/>
@@ -1296,7 +1521,7 @@
         <v>18</v>
       </c>
       <c r="J13" s="39" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K13" s="40"/>
       <c r="L13" s="40"/>
@@ -1319,7 +1544,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -1336,7 +1561,7 @@
     </row>
     <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>19</v>
@@ -1371,7 +1596,7 @@
     </row>
     <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>19</v>
@@ -1398,7 +1623,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
@@ -1406,7 +1631,7 @@
     </row>
     <row r="18" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>19</v>
@@ -1441,7 +1666,7 @@
     </row>
     <row r="19" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>19</v>
@@ -1476,7 +1701,7 @@
     </row>
     <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>19</v>
@@ -1511,7 +1736,7 @@
     </row>
     <row r="21" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>19</v>
@@ -1561,7 +1786,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -1578,7 +1803,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>19</v>
@@ -1628,7 +1853,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
@@ -1643,9 +1868,9 @@
       <c r="L26" s="17"/>
       <c r="M26" s="17"/>
     </row>
-    <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>19</v>
@@ -1678,79 +1903,41 @@
       <c r="L27" s="13"/>
       <c r="M27" s="14"/>
     </row>
-    <row r="28" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="14"/>
-    </row>
-    <row r="29" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="14"/>
-    </row>
-    <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+    </row>
+    <row r="30" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>19</v>
@@ -1783,7 +1970,7 @@
       <c r="L30" s="13"/>
       <c r="M30" s="14"/>
     </row>
-    <row r="31" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -1800,7 +1987,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -1815,9 +2002,9 @@
       <c r="L32" s="17"/>
       <c r="M32" s="17"/>
     </row>
-    <row r="33" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>22</v>
+    <row r="33" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>19</v>
@@ -1850,9 +2037,9 @@
       <c r="L33" s="13"/>
       <c r="M33" s="14"/>
     </row>
-    <row r="34" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>23</v>
+    <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>19</v>
@@ -1886,179 +2073,783 @@
       <c r="M34" s="14"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+    </row>
+    <row r="37" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="14"/>
+    </row>
+    <row r="38" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="14"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
+    </row>
+    <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J41" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="14"/>
+    </row>
+    <row r="42" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="14"/>
+    </row>
+    <row r="43" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J43" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="14"/>
+    </row>
+    <row r="44" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J44" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="14"/>
+    </row>
+    <row r="45" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="16"/>
+    </row>
+    <row r="46" spans="1:13" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J47" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="14"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J48" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="14"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J49" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="14"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J50" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="14"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J51" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="14"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" s="16"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="16"/>
+      <c r="L52" s="16"/>
+      <c r="M52" s="16"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="17"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="17"/>
+      <c r="L53" s="17"/>
+      <c r="M53" s="17"/>
+    </row>
+    <row r="54" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J54" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K54" s="13"/>
+      <c r="L54" s="13"/>
+      <c r="M54" s="14"/>
+    </row>
+    <row r="55" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J55" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K55" s="13"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="14"/>
+    </row>
+    <row r="56" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J56" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K56" s="13"/>
+      <c r="L56" s="13"/>
+      <c r="M56" s="14"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A57" s="16"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="16"/>
+      <c r="I57" s="16"/>
+      <c r="J57" s="16"/>
+      <c r="K57" s="16"/>
+      <c r="L57" s="16"/>
+      <c r="M57" s="16"/>
+    </row>
+    <row r="58" spans="1:13" ht="20" x14ac:dyDescent="0.2">
+      <c r="A58" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58" s="25"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
+      <c r="H58" s="25"/>
+      <c r="I58" s="26"/>
+      <c r="J58" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="K58" s="28"/>
+      <c r="L58" s="28"/>
+      <c r="M58" s="29"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J35" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="14"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="16"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="16"/>
-      <c r="L36" s="16"/>
-      <c r="M36" s="16"/>
-    </row>
-    <row r="37" spans="1:13" ht="20" x14ac:dyDescent="0.2">
-      <c r="A37" s="24" t="s">
+      <c r="C59" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="K37" s="28"/>
-      <c r="L37" s="28"/>
-      <c r="M37" s="29"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="F59" s="30"/>
+      <c r="G59" s="31"/>
+      <c r="H59" s="31"/>
+      <c r="I59" s="31"/>
+      <c r="J59" s="31"/>
+      <c r="K59" s="32"/>
+    </row>
+    <row r="60" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A60" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="B60" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F38" s="30"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="31"/>
-      <c r="K38" s="32"/>
-    </row>
-    <row r="39" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
+      <c r="F60" s="18"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="20"/>
+      <c r="J60" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E39" s="4" t="s">
+      <c r="K60" s="34"/>
+      <c r="L60" s="34"/>
+      <c r="M60" s="35"/>
+    </row>
+    <row r="61" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F39" s="18"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="K39" s="34"/>
-      <c r="L39" s="34"/>
-      <c r="M39" s="35"/>
-    </row>
-    <row r="40" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F40" s="21"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="K40" s="34"/>
-      <c r="L40" s="34"/>
-      <c r="M40" s="35"/>
+      <c r="B61" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F61" s="21"/>
+      <c r="G61" s="22"/>
+      <c r="H61" s="22"/>
+      <c r="I61" s="23"/>
+      <c r="J61" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="K61" s="34"/>
+      <c r="L61" s="34"/>
+      <c r="M61" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="69">
+    <mergeCell ref="J49:M49"/>
+    <mergeCell ref="J47:M47"/>
+    <mergeCell ref="J50:M50"/>
+    <mergeCell ref="J51:M51"/>
+    <mergeCell ref="J48:M48"/>
+    <mergeCell ref="A22:M22"/>
+    <mergeCell ref="A23:M23"/>
+    <mergeCell ref="A26:M26"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="A29:M29"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="A31:M31"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="A32:M32"/>
+    <mergeCell ref="J33:M33"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="A35:M35"/>
     <mergeCell ref="J19:M19"/>
     <mergeCell ref="J20:M20"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:I7"/>
     <mergeCell ref="J6:M7"/>
     <mergeCell ref="J18:M18"/>
-    <mergeCell ref="F39:I40"/>
-    <mergeCell ref="A32:M32"/>
-    <mergeCell ref="J33:M33"/>
-    <mergeCell ref="J34:M34"/>
-    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="F60:I61"/>
+    <mergeCell ref="A53:M53"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="J55:M55"/>
+    <mergeCell ref="J56:M56"/>
+    <mergeCell ref="A57:M57"/>
+    <mergeCell ref="A58:I58"/>
+    <mergeCell ref="J58:M58"/>
+    <mergeCell ref="F59:K59"/>
+    <mergeCell ref="J60:M60"/>
+    <mergeCell ref="J61:M61"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="A52:M52"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="A39:M39"/>
+    <mergeCell ref="A40:M40"/>
+    <mergeCell ref="J41:M41"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="A25:M25"/>
+    <mergeCell ref="A28:M28"/>
     <mergeCell ref="A36:M36"/>
-    <mergeCell ref="A37:I37"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="F38:K38"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="A31:M31"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="A25:M25"/>
-    <mergeCell ref="A26:M26"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="A22:M22"/>
-    <mergeCell ref="A23:M23"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="A45:M45"/>
+    <mergeCell ref="A46:M46"/>
     <mergeCell ref="J17:M17"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:I9"/>
@@ -2080,40 +2871,139 @@
     <mergeCell ref="B2:I3"/>
     <mergeCell ref="J2:M3"/>
   </mergeCells>
-  <conditionalFormatting sqref="B12:I13 B39:E40 B16:I21">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+  <conditionalFormatting sqref="B12:I13 B60:E61 B16:I21">
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
       <formula>"Poor"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
       <formula>"Fair"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="42" operator="equal">
       <formula>"Good"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27:I30">
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+  <conditionalFormatting sqref="B41:I44">
+    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
       <formula>"Poor"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
       <formula>"Fair"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
       <formula>"Good"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B33:I35">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+  <conditionalFormatting sqref="B54:I56">
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
       <formula>"Poor"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
       <formula>"Fair"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
+      <formula>"Good"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38:I38">
+    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
+      <formula>"Poor"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
+      <formula>"Fair"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
+      <formula>"Good"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47:I47 B50:I51">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
+      <formula>"Poor"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+      <formula>"Fair"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
+      <formula>"Good"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48:I48">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+      <formula>"Poor"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+      <formula>"Fair"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
       <formula>"Good"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:I24">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+      <formula>"Poor"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+      <formula>"Fair"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
+      <formula>"Good"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27:I27">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+      <formula>"Poor"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+      <formula>"Fair"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+      <formula>"Good"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30:I30">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>"Poor"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>"Fair"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+      <formula>"Good"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37:I37">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>"Poor"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"Fair"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+      <formula>"Good"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34:I34">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>"Poor"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"Fair"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+      <formula>"Good"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33:I33">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"Poor"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"Fair"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"Good"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49:I49">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Poor"</formula>
     </cfRule>

</xml_diff>

<commit_message>
expanding manual testing section
</commit_message>
<xml_diff>
--- a/BoardgameNerd/test/manualTests.xlsx
+++ b/BoardgameNerd/test/manualTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierluca/personal local/Work/Learn/CodeInstitute/workspace/BoardgameNerd/BoardgameNerd/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3474DB-D9A0-7949-8D6D-DB2196DEC24D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5D86BC-D6C8-F041-A3B7-42980384F0BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="17540" xr2:uid="{3B2D3A10-B4C2-C143-A6C2-842FD9F46DA7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="64">
   <si>
     <t>Validations</t>
   </si>
@@ -322,12 +322,28 @@
   <si>
     <t>empty collections are showing messages</t>
   </si>
+  <si>
+    <r>
+      <t>Checked on</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://pep8online.com/</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -360,6 +376,14 @@
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1235,8 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A56C59-A709-824B-A8C0-8BBDF3C895BA}">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1376,7 +1400,7 @@
         <v>45</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>

</xml_diff>